<commit_message>
Data: Statistical Neighbours updated, along with banner message.
</commit_message>
<xml_diff>
--- a/01_data/02_prod/sn_april_2021.xlsx
+++ b/01_data/02_prod/sn_april_2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtufts\Documents\no_net_work\Open source\local-authority-interactive-tool\01_data\02_prod\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/andrea_stoker_education_gov_uk/Documents/LAIT Shiny Code/local-authority-interactive-tool/01_data/02_prod/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DC6C4B3-1FB4-48D2-B16F-F653407A8DF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{4DC6C4B3-1FB4-48D2-B16F-F653407A8DF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A450A495-51C2-4630-B26C-A94C7611EA44}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{3AED49FA-47EC-457E-9C5A-1E49E6CBC2EA}"/>
+    <workbookView xWindow="-41130" yWindow="-1215" windowWidth="21600" windowHeight="11175" xr2:uid="{3AED49FA-47EC-457E-9C5A-1E49E6CBC2EA}"/>
   </bookViews>
   <sheets>
     <sheet name="LA SN Groups" sheetId="1" r:id="rId1"/>
@@ -1035,42 +1035,42 @@
   </sheetPr>
   <dimension ref="A1:Z164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="B97" sqref="B97"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F162" sqref="F162"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="3"/>
-    <col min="2" max="2" width="28.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="28.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.1796875" style="3" customWidth="1"/>
-    <col min="17" max="17" width="15.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="4.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="4.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="15.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="5.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="27" max="16384" width="9.1796875" style="3"/>
+    <col min="6" max="6" width="9.85546875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" style="3" customWidth="1"/>
+    <col min="11" max="11" width="15.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" style="3" customWidth="1"/>
+    <col min="17" max="17" width="15.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="4.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="27" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1147,7 +1147,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:26" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1224,7 +1224,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -1302,7 +1302,7 @@
       </c>
       <c r="Z3" s="2"/>
     </row>
-    <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>201</v>
       </c>
@@ -1380,7 +1380,7 @@
       </c>
       <c r="Z4" s="6"/>
     </row>
-    <row r="5" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>202</v>
       </c>
@@ -1460,7 +1460,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>203</v>
       </c>
@@ -1540,7 +1540,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>204</v>
       </c>
@@ -1620,7 +1620,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>205</v>
       </c>
@@ -1700,7 +1700,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>206</v>
       </c>
@@ -1780,7 +1780,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>207</v>
       </c>
@@ -1860,7 +1860,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>208</v>
       </c>
@@ -1940,7 +1940,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>209</v>
       </c>
@@ -2020,7 +2020,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>210</v>
       </c>
@@ -2100,7 +2100,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>211</v>
       </c>
@@ -2180,7 +2180,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>212</v>
       </c>
@@ -2260,7 +2260,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>213</v>
       </c>
@@ -2340,7 +2340,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>301</v>
       </c>
@@ -2420,7 +2420,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>302</v>
       </c>
@@ -2500,7 +2500,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <v>303</v>
       </c>
@@ -2580,7 +2580,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>304</v>
       </c>
@@ -2660,7 +2660,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <v>305</v>
       </c>
@@ -2740,7 +2740,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
         <v>306</v>
       </c>
@@ -2820,7 +2820,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
         <v>307</v>
       </c>
@@ -2900,7 +2900,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <v>308</v>
       </c>
@@ -2980,7 +2980,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
         <v>309</v>
       </c>
@@ -3060,7 +3060,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
         <v>310</v>
       </c>
@@ -3140,7 +3140,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
         <v>311</v>
       </c>
@@ -3220,7 +3220,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
         <v>312</v>
       </c>
@@ -3300,7 +3300,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
         <v>313</v>
       </c>
@@ -3380,7 +3380,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
         <v>314</v>
       </c>
@@ -3460,7 +3460,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
         <v>315</v>
       </c>
@@ -3540,7 +3540,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
         <v>316</v>
       </c>
@@ -3620,7 +3620,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4">
         <v>317</v>
       </c>
@@ -3700,7 +3700,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
         <v>318</v>
       </c>
@@ -3780,7 +3780,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4">
         <v>319</v>
       </c>
@@ -3860,7 +3860,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="4">
         <v>320</v>
       </c>
@@ -3940,7 +3940,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="4">
         <v>330</v>
       </c>
@@ -4020,7 +4020,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
         <v>331</v>
       </c>
@@ -4100,7 +4100,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="4">
         <v>332</v>
       </c>
@@ -4180,7 +4180,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="4">
         <v>333</v>
       </c>
@@ -4260,7 +4260,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="4">
         <v>334</v>
       </c>
@@ -4340,7 +4340,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="4">
         <v>335</v>
       </c>
@@ -4420,7 +4420,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="4">
         <v>336</v>
       </c>
@@ -4500,7 +4500,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="4">
         <v>340</v>
       </c>
@@ -4580,7 +4580,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="4">
         <v>341</v>
       </c>
@@ -4660,7 +4660,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="4">
         <v>342</v>
       </c>
@@ -4740,7 +4740,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="47" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="4">
         <v>343</v>
       </c>
@@ -4820,7 +4820,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="48" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="4">
         <v>344</v>
       </c>
@@ -4900,7 +4900,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="4">
         <v>350</v>
       </c>
@@ -4980,7 +4980,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="50" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="4">
         <v>351</v>
       </c>
@@ -5060,7 +5060,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="51" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="4">
         <v>352</v>
       </c>
@@ -5140,7 +5140,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="52" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="4">
         <v>353</v>
       </c>
@@ -5220,7 +5220,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="53" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="4">
         <v>354</v>
       </c>
@@ -5300,7 +5300,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="54" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="4">
         <v>355</v>
       </c>
@@ -5380,7 +5380,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="55" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="4">
         <v>356</v>
       </c>
@@ -5460,7 +5460,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="56" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="4">
         <v>357</v>
       </c>
@@ -5540,7 +5540,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="57" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="4">
         <v>358</v>
       </c>
@@ -5620,7 +5620,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="4">
         <v>359</v>
       </c>
@@ -5700,7 +5700,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="59" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="4">
         <v>370</v>
       </c>
@@ -5780,7 +5780,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="60" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="4">
         <v>371</v>
       </c>
@@ -5860,7 +5860,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="61" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="4">
         <v>372</v>
       </c>
@@ -5940,7 +5940,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="62" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="4">
         <v>373</v>
       </c>
@@ -6020,7 +6020,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="63" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="4">
         <v>380</v>
       </c>
@@ -6100,7 +6100,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="64" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="4">
         <v>381</v>
       </c>
@@ -6180,7 +6180,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="65" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="4">
         <v>382</v>
       </c>
@@ -6260,7 +6260,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="66" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="4">
         <v>383</v>
       </c>
@@ -6340,7 +6340,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="67" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="4">
         <v>384</v>
       </c>
@@ -6420,7 +6420,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="68" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="4">
         <v>390</v>
       </c>
@@ -6500,7 +6500,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="69" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="4">
         <v>391</v>
       </c>
@@ -6580,7 +6580,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="70" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="4">
         <v>392</v>
       </c>
@@ -6660,7 +6660,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="71" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="4">
         <v>393</v>
       </c>
@@ -6740,7 +6740,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="72" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="4">
         <v>394</v>
       </c>
@@ -6820,7 +6820,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="73" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="4">
         <v>420</v>
       </c>
@@ -6900,7 +6900,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="74" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="4">
         <v>800</v>
       </c>
@@ -6980,7 +6980,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="75" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="4">
         <v>801</v>
       </c>
@@ -7060,7 +7060,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="76" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="4">
         <v>802</v>
       </c>
@@ -7140,7 +7140,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="77" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="4">
         <v>803</v>
       </c>
@@ -7220,7 +7220,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="78" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="4">
         <v>805</v>
       </c>
@@ -7300,7 +7300,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="79" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="4">
         <v>806</v>
       </c>
@@ -7380,7 +7380,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="80" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="4">
         <v>807</v>
       </c>
@@ -7460,7 +7460,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="81" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="4">
         <v>808</v>
       </c>
@@ -7540,7 +7540,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="82" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="4">
         <v>810</v>
       </c>
@@ -7620,7 +7620,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="83" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="4">
         <v>811</v>
       </c>
@@ -7700,7 +7700,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="84" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="4">
         <v>812</v>
       </c>
@@ -7780,7 +7780,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="85" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="4">
         <v>813</v>
       </c>
@@ -7860,7 +7860,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="86" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="4">
         <v>815</v>
       </c>
@@ -7940,7 +7940,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="87" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="4">
         <v>816</v>
       </c>
@@ -8020,7 +8020,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="88" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="4">
         <v>821</v>
       </c>
@@ -8100,7 +8100,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="89" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="4">
         <v>822</v>
       </c>
@@ -8178,7 +8178,7 @@
       </c>
       <c r="Z89" s="4"/>
     </row>
-    <row r="90" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="4">
         <v>823</v>
       </c>
@@ -8256,7 +8256,7 @@
       </c>
       <c r="Z90" s="4"/>
     </row>
-    <row r="91" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="4">
         <v>825</v>
       </c>
@@ -8336,7 +8336,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="92" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="4">
         <v>826</v>
       </c>
@@ -8416,7 +8416,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="93" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="4">
         <v>830</v>
       </c>
@@ -8496,7 +8496,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="94" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="4">
         <v>831</v>
       </c>
@@ -8576,7 +8576,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="95" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="3">
         <v>838</v>
       </c>
@@ -8653,7 +8653,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="96" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="3">
         <v>839</v>
       </c>
@@ -8730,7 +8730,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="97" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="3">
         <v>840</v>
       </c>
@@ -8807,7 +8807,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="98" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="4">
         <v>841</v>
       </c>
@@ -8885,7 +8885,7 @@
       </c>
       <c r="Z98" s="4"/>
     </row>
-    <row r="99" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="4">
         <v>845</v>
       </c>
@@ -8963,7 +8963,7 @@
       </c>
       <c r="Z99" s="4"/>
     </row>
-    <row r="100" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="4">
         <v>846</v>
       </c>
@@ -9043,7 +9043,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="101" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="4">
         <v>850</v>
       </c>
@@ -9123,7 +9123,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="102" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="4">
         <v>851</v>
       </c>
@@ -9203,7 +9203,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="103" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="4">
         <v>852</v>
       </c>
@@ -9283,7 +9283,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="104" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="4">
         <v>855</v>
       </c>
@@ -9363,7 +9363,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="105" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="4">
         <v>856</v>
       </c>
@@ -9443,7 +9443,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="106" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="4">
         <v>857</v>
       </c>
@@ -9523,7 +9523,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="107" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="4">
         <v>860</v>
       </c>
@@ -9603,7 +9603,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="108" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="4">
         <v>861</v>
       </c>
@@ -9683,7 +9683,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="109" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="4">
         <v>865</v>
       </c>
@@ -9763,7 +9763,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="110" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="4">
         <v>866</v>
       </c>
@@ -9843,7 +9843,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="111" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="4">
         <v>867</v>
       </c>
@@ -9923,7 +9923,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="112" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="4">
         <v>868</v>
       </c>
@@ -10003,7 +10003,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="113" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="4">
         <v>869</v>
       </c>
@@ -10083,7 +10083,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="114" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="4">
         <v>870</v>
       </c>
@@ -10163,7 +10163,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="115" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="4">
         <v>871</v>
       </c>
@@ -10243,7 +10243,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="116" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="4">
         <v>872</v>
       </c>
@@ -10323,7 +10323,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="117" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="4">
         <v>873</v>
       </c>
@@ -10403,7 +10403,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="118" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="4">
         <v>874</v>
       </c>
@@ -10483,7 +10483,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="119" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="4">
         <v>876</v>
       </c>
@@ -10563,7 +10563,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="120" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="4">
         <v>877</v>
       </c>
@@ -10643,7 +10643,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="121" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="4">
         <v>878</v>
       </c>
@@ -10723,7 +10723,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="122" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="4">
         <v>879</v>
       </c>
@@ -10803,7 +10803,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="123" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="4">
         <v>880</v>
       </c>
@@ -10883,7 +10883,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="124" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="4">
         <v>881</v>
       </c>
@@ -10963,7 +10963,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="125" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="4">
         <v>882</v>
       </c>
@@ -11043,7 +11043,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="126" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="4">
         <v>883</v>
       </c>
@@ -11123,7 +11123,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="127" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="4">
         <v>884</v>
       </c>
@@ -11203,7 +11203,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="128" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="4">
         <v>885</v>
       </c>
@@ -11283,7 +11283,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="129" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="4">
         <v>886</v>
       </c>
@@ -11363,7 +11363,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="130" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="4">
         <v>887</v>
       </c>
@@ -11443,7 +11443,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="131" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="4">
         <v>888</v>
       </c>
@@ -11523,7 +11523,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="132" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="4">
         <v>889</v>
       </c>
@@ -11603,7 +11603,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="133" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="4">
         <v>890</v>
       </c>
@@ -11683,7 +11683,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="134" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="4">
         <v>891</v>
       </c>
@@ -11763,7 +11763,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="135" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="4">
         <v>892</v>
       </c>
@@ -11843,7 +11843,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="136" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="4">
         <v>893</v>
       </c>
@@ -11923,7 +11923,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="137" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="4">
         <v>894</v>
       </c>
@@ -12003,7 +12003,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="138" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="4">
         <v>895</v>
       </c>
@@ -12083,7 +12083,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="139" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="4">
         <v>896</v>
       </c>
@@ -12163,7 +12163,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="140" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="4">
         <v>908</v>
       </c>
@@ -12243,7 +12243,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="141" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="4">
         <v>909</v>
       </c>
@@ -12321,7 +12321,7 @@
       </c>
       <c r="Z141" s="4"/>
     </row>
-    <row r="142" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="4">
         <v>916</v>
       </c>
@@ -12399,7 +12399,7 @@
       </c>
       <c r="Z142" s="4"/>
     </row>
-    <row r="143" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="4">
         <v>919</v>
       </c>
@@ -12479,7 +12479,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="144" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="4">
         <v>921</v>
       </c>
@@ -12559,7 +12559,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="145" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="4">
         <v>925</v>
       </c>
@@ -12639,7 +12639,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="146" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="4">
         <v>926</v>
       </c>
@@ -12719,7 +12719,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="147" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="4">
         <v>929</v>
       </c>
@@ -12799,7 +12799,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="148" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="4">
         <v>931</v>
       </c>
@@ -12879,7 +12879,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="149" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="4">
         <v>933</v>
       </c>
@@ -12959,7 +12959,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="150" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="4">
         <v>935</v>
       </c>
@@ -13039,7 +13039,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="151" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="4">
         <v>936</v>
       </c>
@@ -13119,7 +13119,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="152" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="4">
         <v>937</v>
       </c>
@@ -13199,7 +13199,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="153" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="4">
         <v>938</v>
       </c>
@@ -13279,7 +13279,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="154" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="3">
         <v>940</v>
       </c>
@@ -13356,7 +13356,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="155" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="3">
         <v>941</v>
       </c>
@@ -13433,7 +13433,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="156" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="7">
         <v>942</v>
       </c>
@@ -13510,7 +13510,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="157" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="7">
         <v>943</v>
       </c>
@@ -13587,12 +13587,12 @@
         <v>189</v>
       </c>
     </row>
-    <row r="159" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B159" s="3" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="161" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="4">
         <v>835</v>
       </c>
@@ -13672,7 +13672,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="162" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="4">
         <v>836</v>
       </c>
@@ -13752,7 +13752,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="163" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="4">
         <v>837</v>
       </c>
@@ -13832,7 +13832,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="164" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="4">
         <v>928</v>
       </c>

</xml_diff>

<commit_message>
Data: Statistical Neighbours updated, along with banner message. (#92)
* Data: Statistical Neighbours updated, along with banner message.

* Revised SVGlite version

* SVGlite version moved to 2.2.1

---------

Co-authored-by: STOKER <Andrea.STOKER@EDUCATION.GOV.UK>
</commit_message>
<xml_diff>
--- a/01_data/02_prod/sn_april_2021.xlsx
+++ b/01_data/02_prod/sn_april_2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtufts\Documents\no_net_work\Open source\local-authority-interactive-tool\01_data\02_prod\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/andrea_stoker_education_gov_uk/Documents/LAIT Shiny Code/local-authority-interactive-tool/01_data/02_prod/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DC6C4B3-1FB4-48D2-B16F-F653407A8DF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{4DC6C4B3-1FB4-48D2-B16F-F653407A8DF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A450A495-51C2-4630-B26C-A94C7611EA44}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{3AED49FA-47EC-457E-9C5A-1E49E6CBC2EA}"/>
+    <workbookView xWindow="-41130" yWindow="-1215" windowWidth="21600" windowHeight="11175" xr2:uid="{3AED49FA-47EC-457E-9C5A-1E49E6CBC2EA}"/>
   </bookViews>
   <sheets>
     <sheet name="LA SN Groups" sheetId="1" r:id="rId1"/>
@@ -1035,42 +1035,42 @@
   </sheetPr>
   <dimension ref="A1:Z164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="B97" sqref="B97"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F162" sqref="F162"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="3"/>
-    <col min="2" max="2" width="28.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="28.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.1796875" style="3" customWidth="1"/>
-    <col min="17" max="17" width="15.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="4.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="4.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="15.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="5.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="27" max="16384" width="9.1796875" style="3"/>
+    <col min="6" max="6" width="9.85546875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" style="3" customWidth="1"/>
+    <col min="11" max="11" width="15.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" style="3" customWidth="1"/>
+    <col min="17" max="17" width="15.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="4.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="27" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1147,7 +1147,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:26" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1224,7 +1224,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -1302,7 +1302,7 @@
       </c>
       <c r="Z3" s="2"/>
     </row>
-    <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>201</v>
       </c>
@@ -1380,7 +1380,7 @@
       </c>
       <c r="Z4" s="6"/>
     </row>
-    <row r="5" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>202</v>
       </c>
@@ -1460,7 +1460,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>203</v>
       </c>
@@ -1540,7 +1540,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>204</v>
       </c>
@@ -1620,7 +1620,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>205</v>
       </c>
@@ -1700,7 +1700,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>206</v>
       </c>
@@ -1780,7 +1780,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>207</v>
       </c>
@@ -1860,7 +1860,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>208</v>
       </c>
@@ -1940,7 +1940,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>209</v>
       </c>
@@ -2020,7 +2020,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>210</v>
       </c>
@@ -2100,7 +2100,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>211</v>
       </c>
@@ -2180,7 +2180,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>212</v>
       </c>
@@ -2260,7 +2260,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>213</v>
       </c>
@@ -2340,7 +2340,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>301</v>
       </c>
@@ -2420,7 +2420,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>302</v>
       </c>
@@ -2500,7 +2500,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <v>303</v>
       </c>
@@ -2580,7 +2580,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>304</v>
       </c>
@@ -2660,7 +2660,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <v>305</v>
       </c>
@@ -2740,7 +2740,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
         <v>306</v>
       </c>
@@ -2820,7 +2820,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
         <v>307</v>
       </c>
@@ -2900,7 +2900,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <v>308</v>
       </c>
@@ -2980,7 +2980,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
         <v>309</v>
       </c>
@@ -3060,7 +3060,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
         <v>310</v>
       </c>
@@ -3140,7 +3140,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
         <v>311</v>
       </c>
@@ -3220,7 +3220,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
         <v>312</v>
       </c>
@@ -3300,7 +3300,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
         <v>313</v>
       </c>
@@ -3380,7 +3380,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
         <v>314</v>
       </c>
@@ -3460,7 +3460,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
         <v>315</v>
       </c>
@@ -3540,7 +3540,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
         <v>316</v>
       </c>
@@ -3620,7 +3620,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4">
         <v>317</v>
       </c>
@@ -3700,7 +3700,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
         <v>318</v>
       </c>
@@ -3780,7 +3780,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4">
         <v>319</v>
       </c>
@@ -3860,7 +3860,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="4">
         <v>320</v>
       </c>
@@ -3940,7 +3940,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="4">
         <v>330</v>
       </c>
@@ -4020,7 +4020,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
         <v>331</v>
       </c>
@@ -4100,7 +4100,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="4">
         <v>332</v>
       </c>
@@ -4180,7 +4180,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="4">
         <v>333</v>
       </c>
@@ -4260,7 +4260,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="4">
         <v>334</v>
       </c>
@@ -4340,7 +4340,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="4">
         <v>335</v>
       </c>
@@ -4420,7 +4420,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="4">
         <v>336</v>
       </c>
@@ -4500,7 +4500,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="4">
         <v>340</v>
       </c>
@@ -4580,7 +4580,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="4">
         <v>341</v>
       </c>
@@ -4660,7 +4660,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="4">
         <v>342</v>
       </c>
@@ -4740,7 +4740,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="47" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="4">
         <v>343</v>
       </c>
@@ -4820,7 +4820,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="48" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="4">
         <v>344</v>
       </c>
@@ -4900,7 +4900,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="4">
         <v>350</v>
       </c>
@@ -4980,7 +4980,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="50" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="4">
         <v>351</v>
       </c>
@@ -5060,7 +5060,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="51" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="4">
         <v>352</v>
       </c>
@@ -5140,7 +5140,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="52" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="4">
         <v>353</v>
       </c>
@@ -5220,7 +5220,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="53" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="4">
         <v>354</v>
       </c>
@@ -5300,7 +5300,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="54" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="4">
         <v>355</v>
       </c>
@@ -5380,7 +5380,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="55" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="4">
         <v>356</v>
       </c>
@@ -5460,7 +5460,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="56" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="4">
         <v>357</v>
       </c>
@@ -5540,7 +5540,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="57" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="4">
         <v>358</v>
       </c>
@@ -5620,7 +5620,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="4">
         <v>359</v>
       </c>
@@ -5700,7 +5700,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="59" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="4">
         <v>370</v>
       </c>
@@ -5780,7 +5780,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="60" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="4">
         <v>371</v>
       </c>
@@ -5860,7 +5860,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="61" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="4">
         <v>372</v>
       </c>
@@ -5940,7 +5940,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="62" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="4">
         <v>373</v>
       </c>
@@ -6020,7 +6020,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="63" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="4">
         <v>380</v>
       </c>
@@ -6100,7 +6100,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="64" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="4">
         <v>381</v>
       </c>
@@ -6180,7 +6180,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="65" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="4">
         <v>382</v>
       </c>
@@ -6260,7 +6260,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="66" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="4">
         <v>383</v>
       </c>
@@ -6340,7 +6340,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="67" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="4">
         <v>384</v>
       </c>
@@ -6420,7 +6420,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="68" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="4">
         <v>390</v>
       </c>
@@ -6500,7 +6500,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="69" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="4">
         <v>391</v>
       </c>
@@ -6580,7 +6580,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="70" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="4">
         <v>392</v>
       </c>
@@ -6660,7 +6660,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="71" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="4">
         <v>393</v>
       </c>
@@ -6740,7 +6740,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="72" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="4">
         <v>394</v>
       </c>
@@ -6820,7 +6820,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="73" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="4">
         <v>420</v>
       </c>
@@ -6900,7 +6900,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="74" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="4">
         <v>800</v>
       </c>
@@ -6980,7 +6980,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="75" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="4">
         <v>801</v>
       </c>
@@ -7060,7 +7060,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="76" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="4">
         <v>802</v>
       </c>
@@ -7140,7 +7140,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="77" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="4">
         <v>803</v>
       </c>
@@ -7220,7 +7220,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="78" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="4">
         <v>805</v>
       </c>
@@ -7300,7 +7300,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="79" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="4">
         <v>806</v>
       </c>
@@ -7380,7 +7380,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="80" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="4">
         <v>807</v>
       </c>
@@ -7460,7 +7460,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="81" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="4">
         <v>808</v>
       </c>
@@ -7540,7 +7540,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="82" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="4">
         <v>810</v>
       </c>
@@ -7620,7 +7620,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="83" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="4">
         <v>811</v>
       </c>
@@ -7700,7 +7700,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="84" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="4">
         <v>812</v>
       </c>
@@ -7780,7 +7780,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="85" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="4">
         <v>813</v>
       </c>
@@ -7860,7 +7860,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="86" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="4">
         <v>815</v>
       </c>
@@ -7940,7 +7940,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="87" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="4">
         <v>816</v>
       </c>
@@ -8020,7 +8020,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="88" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="4">
         <v>821</v>
       </c>
@@ -8100,7 +8100,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="89" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="4">
         <v>822</v>
       </c>
@@ -8178,7 +8178,7 @@
       </c>
       <c r="Z89" s="4"/>
     </row>
-    <row r="90" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="4">
         <v>823</v>
       </c>
@@ -8256,7 +8256,7 @@
       </c>
       <c r="Z90" s="4"/>
     </row>
-    <row r="91" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="4">
         <v>825</v>
       </c>
@@ -8336,7 +8336,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="92" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="4">
         <v>826</v>
       </c>
@@ -8416,7 +8416,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="93" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="4">
         <v>830</v>
       </c>
@@ -8496,7 +8496,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="94" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="4">
         <v>831</v>
       </c>
@@ -8576,7 +8576,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="95" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="3">
         <v>838</v>
       </c>
@@ -8653,7 +8653,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="96" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="3">
         <v>839</v>
       </c>
@@ -8730,7 +8730,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="97" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="3">
         <v>840</v>
       </c>
@@ -8807,7 +8807,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="98" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="4">
         <v>841</v>
       </c>
@@ -8885,7 +8885,7 @@
       </c>
       <c r="Z98" s="4"/>
     </row>
-    <row r="99" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="4">
         <v>845</v>
       </c>
@@ -8963,7 +8963,7 @@
       </c>
       <c r="Z99" s="4"/>
     </row>
-    <row r="100" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="4">
         <v>846</v>
       </c>
@@ -9043,7 +9043,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="101" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="4">
         <v>850</v>
       </c>
@@ -9123,7 +9123,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="102" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="4">
         <v>851</v>
       </c>
@@ -9203,7 +9203,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="103" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="4">
         <v>852</v>
       </c>
@@ -9283,7 +9283,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="104" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="4">
         <v>855</v>
       </c>
@@ -9363,7 +9363,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="105" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="4">
         <v>856</v>
       </c>
@@ -9443,7 +9443,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="106" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="4">
         <v>857</v>
       </c>
@@ -9523,7 +9523,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="107" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="4">
         <v>860</v>
       </c>
@@ -9603,7 +9603,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="108" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="4">
         <v>861</v>
       </c>
@@ -9683,7 +9683,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="109" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="4">
         <v>865</v>
       </c>
@@ -9763,7 +9763,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="110" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="4">
         <v>866</v>
       </c>
@@ -9843,7 +9843,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="111" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="4">
         <v>867</v>
       </c>
@@ -9923,7 +9923,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="112" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="4">
         <v>868</v>
       </c>
@@ -10003,7 +10003,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="113" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="4">
         <v>869</v>
       </c>
@@ -10083,7 +10083,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="114" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="4">
         <v>870</v>
       </c>
@@ -10163,7 +10163,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="115" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="4">
         <v>871</v>
       </c>
@@ -10243,7 +10243,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="116" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="4">
         <v>872</v>
       </c>
@@ -10323,7 +10323,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="117" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="4">
         <v>873</v>
       </c>
@@ -10403,7 +10403,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="118" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="4">
         <v>874</v>
       </c>
@@ -10483,7 +10483,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="119" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="4">
         <v>876</v>
       </c>
@@ -10563,7 +10563,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="120" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="4">
         <v>877</v>
       </c>
@@ -10643,7 +10643,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="121" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="4">
         <v>878</v>
       </c>
@@ -10723,7 +10723,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="122" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="4">
         <v>879</v>
       </c>
@@ -10803,7 +10803,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="123" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="4">
         <v>880</v>
       </c>
@@ -10883,7 +10883,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="124" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="4">
         <v>881</v>
       </c>
@@ -10963,7 +10963,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="125" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="4">
         <v>882</v>
       </c>
@@ -11043,7 +11043,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="126" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="4">
         <v>883</v>
       </c>
@@ -11123,7 +11123,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="127" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="4">
         <v>884</v>
       </c>
@@ -11203,7 +11203,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="128" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="4">
         <v>885</v>
       </c>
@@ -11283,7 +11283,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="129" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="4">
         <v>886</v>
       </c>
@@ -11363,7 +11363,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="130" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="4">
         <v>887</v>
       </c>
@@ -11443,7 +11443,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="131" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="4">
         <v>888</v>
       </c>
@@ -11523,7 +11523,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="132" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="4">
         <v>889</v>
       </c>
@@ -11603,7 +11603,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="133" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="4">
         <v>890</v>
       </c>
@@ -11683,7 +11683,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="134" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="4">
         <v>891</v>
       </c>
@@ -11763,7 +11763,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="135" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="4">
         <v>892</v>
       </c>
@@ -11843,7 +11843,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="136" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="4">
         <v>893</v>
       </c>
@@ -11923,7 +11923,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="137" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="4">
         <v>894</v>
       </c>
@@ -12003,7 +12003,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="138" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="4">
         <v>895</v>
       </c>
@@ -12083,7 +12083,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="139" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="4">
         <v>896</v>
       </c>
@@ -12163,7 +12163,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="140" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="4">
         <v>908</v>
       </c>
@@ -12243,7 +12243,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="141" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="4">
         <v>909</v>
       </c>
@@ -12321,7 +12321,7 @@
       </c>
       <c r="Z141" s="4"/>
     </row>
-    <row r="142" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="4">
         <v>916</v>
       </c>
@@ -12399,7 +12399,7 @@
       </c>
       <c r="Z142" s="4"/>
     </row>
-    <row r="143" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="4">
         <v>919</v>
       </c>
@@ -12479,7 +12479,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="144" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="4">
         <v>921</v>
       </c>
@@ -12559,7 +12559,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="145" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="4">
         <v>925</v>
       </c>
@@ -12639,7 +12639,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="146" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="4">
         <v>926</v>
       </c>
@@ -12719,7 +12719,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="147" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="4">
         <v>929</v>
       </c>
@@ -12799,7 +12799,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="148" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="4">
         <v>931</v>
       </c>
@@ -12879,7 +12879,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="149" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="4">
         <v>933</v>
       </c>
@@ -12959,7 +12959,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="150" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="4">
         <v>935</v>
       </c>
@@ -13039,7 +13039,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="151" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="4">
         <v>936</v>
       </c>
@@ -13119,7 +13119,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="152" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="4">
         <v>937</v>
       </c>
@@ -13199,7 +13199,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="153" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="4">
         <v>938</v>
       </c>
@@ -13279,7 +13279,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="154" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="3">
         <v>940</v>
       </c>
@@ -13356,7 +13356,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="155" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="3">
         <v>941</v>
       </c>
@@ -13433,7 +13433,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="156" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="7">
         <v>942</v>
       </c>
@@ -13510,7 +13510,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="157" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="7">
         <v>943</v>
       </c>
@@ -13587,12 +13587,12 @@
         <v>189</v>
       </c>
     </row>
-    <row r="159" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B159" s="3" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="161" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="4">
         <v>835</v>
       </c>
@@ -13672,7 +13672,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="162" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="4">
         <v>836</v>
       </c>
@@ -13752,7 +13752,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="163" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="4">
         <v>837</v>
       </c>
@@ -13832,7 +13832,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="164" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="4">
         <v>928</v>
       </c>

</xml_diff>